<commit_message>
correcion detalles auditorias no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2016/1/P1446 - RNCFAC, Juan Carlos Sanchez_AG/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2016/1/P1446 - RNCFAC, Juan Carlos Sanchez_AG/Calidad/No_conformidades.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="No Conformidades" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="No Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>REPORTE DE NO CONFORMIDADES P1446 - RNCFAC, Juan Carlos Sanchez_AG/</t>
   </si>
@@ -66,9 +68,6 @@
   </si>
   <si>
     <t>No existe plan de proyecto</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
   <si>
     <t>No se notifico creacion de linea base</t>
@@ -81,11 +80,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -94,22 +92,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -117,7 +100,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -152,91 +135,94 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -295,36 +281,324 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.8582995951417"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.2793522267206"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2874493927125"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="0" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.5708502024292"/>
+    <col min="1" max="1" width="2.85546875"/>
+    <col min="2" max="2" width="42"/>
+    <col min="3" max="3" width="18.7109375"/>
+    <col min="4" max="4" width="24.28515625"/>
+    <col min="5" max="5" width="16.5703125"/>
+    <col min="6" max="6" width="10.85546875"/>
+    <col min="7" max="7" width="27.28515625"/>
+    <col min="8" max="1023" width="10.85546875"/>
+    <col min="1024" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="15.6" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -335,7 +609,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -344,7 +618,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -367,8 +641,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -377,7 +651,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="5">
         <v>42396</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -390,8 +664,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -400,10 +674,10 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>42399</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="5">
         <v>42401</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -411,8 +685,8 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -421,10 +695,10 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="5">
         <v>42398</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="5">
         <v>42401</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -432,8 +706,8 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -442,29 +716,31 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="5">
         <v>42398</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="7">
+        <v>42404</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="5">
         <v>42398</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="5">
         <v>42401</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -472,20 +748,20 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="3">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="5">
         <v>42398</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="5">
         <v>42401</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -493,8 +769,8 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:7">
+      <c r="A10" s="3">
         <v>13</v>
       </c>
       <c r="B10" s="3"/>
@@ -504,8 +780,8 @@
       <c r="F10" s="6"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:7">
+      <c r="A11" s="3">
         <v>14</v>
       </c>
       <c r="B11" s="3"/>
@@ -515,8 +791,8 @@
       <c r="F11" s="6"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:7">
+      <c r="A12" s="3">
         <v>15</v>
       </c>
       <c r="B12" s="3"/>
@@ -526,8 +802,8 @@
       <c r="F12" s="6"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:7">
+      <c r="A13" s="3">
         <v>16</v>
       </c>
       <c r="B13" s="3"/>
@@ -537,8 +813,8 @@
       <c r="F13" s="6"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:7">
+      <c r="A14" s="3">
         <v>17</v>
       </c>
       <c r="B14" s="3"/>
@@ -548,8 +824,8 @@
       <c r="F14" s="6"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:7">
+      <c r="A15" s="3">
         <v>18</v>
       </c>
       <c r="B15" s="3"/>
@@ -559,8 +835,8 @@
       <c r="F15" s="6"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:7">
+      <c r="A16" s="3">
         <v>19</v>
       </c>
       <c r="B16" s="3"/>
@@ -570,8 +846,8 @@
       <c r="F16" s="6"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:7">
+      <c r="A17" s="3">
         <v>20</v>
       </c>
       <c r="B17" s="3"/>
@@ -581,8 +857,8 @@
       <c r="F17" s="6"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" spans="1:7">
+      <c r="A18" s="3">
         <v>21</v>
       </c>
       <c r="B18" s="3"/>
@@ -592,8 +868,8 @@
       <c r="F18" s="6"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="19" spans="1:7">
+      <c r="A19" s="3">
         <v>22</v>
       </c>
       <c r="B19" s="3"/>
@@ -603,8 +879,8 @@
       <c r="F19" s="6"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="20" spans="1:7">
+      <c r="A20" s="3">
         <v>23</v>
       </c>
       <c r="B20" s="3"/>
@@ -614,8 +890,8 @@
       <c r="F20" s="6"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+    <row r="21" spans="1:7">
+      <c r="A21" s="3">
         <v>24</v>
       </c>
       <c r="B21" s="3"/>
@@ -625,8 +901,8 @@
       <c r="F21" s="6"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="22" spans="1:7">
+      <c r="A22" s="3">
         <v>25</v>
       </c>
       <c r="B22" s="3"/>
@@ -641,17 +917,12 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F22" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F22">
       <formula1>"En proceso,Cerrada,Cancelada,Rechazada"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>